<commit_message>
Resolves feat 1 - 2
</commit_message>
<xml_diff>
--- a/Liste-membres.xlsx
+++ b/Liste-membres.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">53005</t>
   </si>
   <si>
-    <t xml:space="preserve">xxxxx</t>
+    <t xml:space="preserve">xxxxxx</t>
   </si>
   <si>
     <t xml:space="preserve">Saint Hilaire de Loulay</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">04205</t>
   </si>
   <si>
-    <t xml:space="preserve">zzzzz</t>
+    <t xml:space="preserve">zzzzzz</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">74027</t>
   </si>
   <si>
-    <t xml:space="preserve">aaaaa</t>
+    <t xml:space="preserve">aaaaaa</t>
   </si>
 </sst>
 </file>

</xml_diff>